<commit_message>
Added data from Springer COmpact
and recalculated statistics with new presentation. Not finished yet.
</commit_message>
<xml_diff>
--- a/data/gu/apc_gu_2015-2017.xlsx
+++ b/data/gu/apc_gu_2015-2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30260" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -780,8 +780,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -808,24 +815,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1112,7 +1111,7 @@
   <dimension ref="A1:K236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1121,38 +1120,38 @@
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5153,7 +5152,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>